<commit_message>
Fixed some issues with information in the spreed sheet.
</commit_message>
<xml_diff>
--- a/OptClim_lookup.xlsx
+++ b/OptClim_lookup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="6990" windowHeight="6045"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="6996" windowHeight="6048"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="350">
   <si>
     <t>Study Name</t>
   </si>
@@ -1061,6 +1061,9 @@
   </si>
   <si>
     <t>HadCM3\4xCO2\ss4xc</t>
+  </si>
+  <si>
+    <t>Failed -- ctl</t>
   </si>
 </sst>
 </file>
@@ -1409,31 +1412,31 @@
   <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" customWidth="1"/>
-    <col min="7" max="11" width="28.85546875" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" customWidth="1"/>
-    <col min="15" max="15" width="25.140625" customWidth="1"/>
-    <col min="16" max="16" width="55.7109375" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" customWidth="1"/>
+    <col min="7" max="11" width="28.88671875" customWidth="1"/>
+    <col min="12" max="12" width="27.33203125" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" customWidth="1"/>
+    <col min="14" max="14" width="31.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.109375" customWidth="1"/>
+    <col min="16" max="16" width="55.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.109375" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -1554,7 +1557,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>327</v>
       </c>
@@ -1695,7 +1698,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>329</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>328</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1971,12 +1974,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>349</v>
       </c>
       <c r="C12" t="s">
         <v>305</v>
@@ -2006,7 +2009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -2050,7 +2053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -2226,12 +2229,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>349</v>
       </c>
       <c r="C18" t="s">
         <v>305</v>
@@ -2261,7 +2264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2419,7 +2422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2783,7 +2786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2853,7 +2856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>244</v>
       </c>
@@ -2887,17 +2890,17 @@
       <c r="O36" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>252</v>
       </c>
@@ -2931,17 +2934,17 @@
       <c r="O37" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>260</v>
       </c>
@@ -2975,17 +2978,17 @@
       <c r="O38" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>268</v>
       </c>
@@ -3019,17 +3022,17 @@
       <c r="O39" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>276</v>
       </c>
@@ -3063,13 +3066,13 @@
       <c r="O40" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>